<commit_message>
Algorithm working - Need to implement batch imports
</commit_message>
<xml_diff>
--- a/recommended_trades.xlsx
+++ b/recommended_trades.xlsx
@@ -1939,7 +1939,7 @@
         <v>72714960896</v>
       </c>
       <c r="D2" s="3">
-        <v>0</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1953,7 +1953,7 @@
         <v>10744139776</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1967,7 +1967,7 @@
         <v>206312996864</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1981,7 +1981,7 @@
         <v>323528163328</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1995,7 +1995,7 @@
         <v>226429059072</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>548</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2009,7 +2009,7 @@
         <v>227112386560</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>385</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2023,7 +2023,7 @@
         <v>222608965632</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2037,7 +2037,7 @@
         <v>9271792640</v>
       </c>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>15245</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2051,7 +2051,7 @@
         <v>63385825280</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2065,7 +2065,7 @@
         <v>39396507648</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2079,7 +2079,7 @@
         <v>74347970560</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2093,7 +2093,7 @@
         <v>86393380864</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2107,7 +2107,7 @@
         <v>14124343296</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2121,7 +2121,7 @@
         <v>12692014080</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2135,7 +2135,7 @@
         <v>19314720768</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2149,7 +2149,7 @@
         <v>17377003520</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>854</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2163,7 +2163,7 @@
         <v>12292670464</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2177,7 +2177,7 @@
         <v>16317166592</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2191,7 +2191,7 @@
         <v>55132143616</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>958</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2205,7 +2205,7 @@
         <v>2080348962816</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2219,7 +2219,7 @@
         <v>2080335986688</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2233,7 +2233,7 @@
         <v>97858330624</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>3443</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2247,7 +2247,7 @@
         <v>2185963372544</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>956</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2261,7 +2261,7 @@
         <v>15378418688</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
+        <v>18684</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2275,7 +2275,7 @@
         <v>5924403712</v>
       </c>
       <c r="D26" s="3">
-        <v>0</v>
+        <v>8164</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2289,7 +2289,7 @@
         <v>25352775680</v>
       </c>
       <c r="D27" s="3">
-        <v>0</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2303,7 +2303,7 @@
         <v>53197918208</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2317,7 +2317,7 @@
         <v>214630301696</v>
       </c>
       <c r="D29" s="3">
-        <v>0</v>
+        <v>652</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2331,7 +2331,7 @@
         <v>48117575680</v>
       </c>
       <c r="D30" s="3">
-        <v>0</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2345,7 +2345,7 @@
         <v>97803640832</v>
       </c>
       <c r="D31" s="3">
-        <v>0</v>
+        <v>951</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2359,7 +2359,7 @@
         <v>26955816960</v>
       </c>
       <c r="D32" s="3">
-        <v>0</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2373,7 +2373,7 @@
         <v>55683465216</v>
       </c>
       <c r="D33" s="3">
-        <v>0</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2387,7 +2387,7 @@
         <v>45128040448</v>
       </c>
       <c r="D34" s="3">
-        <v>0</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2401,7 +2401,7 @@
         <v>152051957760</v>
       </c>
       <c r="D35" s="3">
-        <v>0</v>
+        <v>702</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2415,7 +2415,7 @@
         <v>87696547840</v>
       </c>
       <c r="D36" s="3">
-        <v>0</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2429,7 +2429,7 @@
         <v>108217556992</v>
       </c>
       <c r="D37" s="3">
-        <v>0</v>
+        <v>911</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2443,7 +2443,7 @@
         <v>30703695872</v>
       </c>
       <c r="D38" s="3">
-        <v>0</v>
+        <v>566</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2457,7 +2457,7 @@
         <v>85059715072</v>
       </c>
       <c r="D39" s="3">
-        <v>0</v>
+        <v>507</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2471,7 +2471,7 @@
         <v>8379299840</v>
       </c>
       <c r="D40" s="3">
-        <v>0</v>
+        <v>8777</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2485,7 +2485,7 @@
         <v>3587432775680</v>
       </c>
       <c r="D41" s="3">
-        <v>0</v>
+        <v>837</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2499,7 +2499,7 @@
         <v>144031629312</v>
       </c>
       <c r="D42" s="3">
-        <v>0</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2513,7 +2513,7 @@
         <v>13051548672</v>
       </c>
       <c r="D43" s="3">
-        <v>0</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2527,7 +2527,7 @@
         <v>37902647296</v>
       </c>
       <c r="D44" s="3">
-        <v>0</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2541,7 +2541,7 @@
         <v>26127955968</v>
       </c>
       <c r="D45" s="3">
-        <v>0</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2555,7 +2555,7 @@
         <v>127808954368</v>
       </c>
       <c r="D46" s="3">
-        <v>0</v>
+        <v>489</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2569,7 +2569,7 @@
         <v>69160534016</v>
       </c>
       <c r="D47" s="3">
-        <v>0</v>
+        <v>636</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2583,7 +2583,7 @@
         <v>11647369216</v>
       </c>
       <c r="D48" s="3">
-        <v>0</v>
+        <v>875</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2597,7 +2597,7 @@
         <v>166969016320</v>
       </c>
       <c r="D49" s="3">
-        <v>0</v>
+        <v>8584</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2611,7 +2611,7 @@
         <v>23532077056</v>
       </c>
       <c r="D50" s="3">
-        <v>0</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2625,7 +2625,7 @@
         <v>62907072512</v>
       </c>
       <c r="D51" s="3">
-        <v>0</v>
+        <v>681</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2639,7 +2639,7 @@
         <v>125060767744</v>
       </c>
       <c r="D52" s="3">
-        <v>0</v>
+        <v>647</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2653,7 +2653,7 @@
         <v>53578854400</v>
       </c>
       <c r="D53" s="3">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2667,7 +2667,7 @@
         <v>33825443840</v>
       </c>
       <c r="D54" s="3">
-        <v>0</v>
+        <v>844</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2681,7 +2681,7 @@
         <v>16547341312</v>
       </c>
       <c r="D55" s="3">
-        <v>0</v>
+        <v>965</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2695,7 +2695,7 @@
         <v>49333805056</v>
       </c>
       <c r="D56" s="3">
-        <v>0</v>
+        <v>307</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2709,7 +2709,7 @@
         <v>43489669120</v>
       </c>
       <c r="D57" s="3">
-        <v>0</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2723,7 +2723,7 @@
         <v>18681440256</v>
       </c>
       <c r="D58" s="3">
-        <v>0</v>
+        <v>3198</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2737,7 +2737,7 @@
         <v>366533443584</v>
       </c>
       <c r="D59" s="3">
-        <v>0</v>
+        <v>4184</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2751,7 +2751,7 @@
         <v>17211920384</v>
       </c>
       <c r="D60" s="3">
-        <v>0</v>
+        <v>5897</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2765,7 +2765,7 @@
         <v>64179245056</v>
       </c>
       <c r="D61" s="3">
-        <v>0</v>
+        <v>895</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2787,7 +2787,7 @@
         <v>19325249536</v>
       </c>
       <c r="D63" s="3">
-        <v>0</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2801,7 +2801,7 @@
         <v>11977266176</v>
       </c>
       <c r="D64" s="3">
-        <v>0</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2815,7 +2815,7 @@
         <v>23406845952</v>
       </c>
       <c r="D65" s="3">
-        <v>0</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2829,7 +2829,7 @@
         <v>151505321984</v>
       </c>
       <c r="D66" s="3">
-        <v>0</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2843,7 +2843,7 @@
         <v>229260230656</v>
       </c>
       <c r="D67" s="3">
-        <v>0</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2857,7 +2857,7 @@
         <v>59525877760</v>
       </c>
       <c r="D68" s="3">
-        <v>0</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2871,7 +2871,7 @@
         <v>116296482816</v>
       </c>
       <c r="D69" s="3">
-        <v>0</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2885,7 +2885,7 @@
         <v>172869074944</v>
       </c>
       <c r="D70" s="3">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2899,7 +2899,7 @@
         <v>7505783808</v>
       </c>
       <c r="D71" s="3">
-        <v>0</v>
+        <v>5792</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2913,7 +2913,7 @@
         <v>133749792768</v>
       </c>
       <c r="D72" s="3">
-        <v>0</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2927,7 +2927,7 @@
         <v>120210087936</v>
       </c>
       <c r="D73" s="3">
-        <v>0</v>
+        <v>3357</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2941,7 +2941,7 @@
         <v>757007646720</v>
       </c>
       <c r="D74" s="3">
-        <v>0</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2955,7 +2955,7 @@
         <v>27588143104</v>
       </c>
       <c r="D75" s="3">
-        <v>0</v>
+        <v>842</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2969,7 +2969,7 @@
         <v>32370464768</v>
       </c>
       <c r="D76" s="3">
-        <v>0</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2991,7 +2991,7 @@
         <v>21459900416</v>
       </c>
       <c r="D78" s="3">
-        <v>0</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -3005,7 +3005,7 @@
         <v>12530127872</v>
       </c>
       <c r="D79" s="3">
-        <v>0</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -3019,7 +3019,7 @@
         <v>14614306816</v>
       </c>
       <c r="D80" s="3">
-        <v>0</v>
+        <v>2424</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -3033,7 +3033,7 @@
         <v>12480083968</v>
       </c>
       <c r="D81" s="3">
-        <v>0</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3047,7 +3047,7 @@
         <v>84146634752</v>
       </c>
       <c r="D82" s="3">
-        <v>0</v>
+        <v>647</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -3061,7 +3061,7 @@
         <v>8178355712</v>
       </c>
       <c r="D83" s="3">
-        <v>0</v>
+        <v>5165</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -3075,7 +3075,7 @@
         <v>13551679488</v>
       </c>
       <c r="D84" s="3">
-        <v>0</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -3089,7 +3089,7 @@
         <v>13749859328</v>
       </c>
       <c r="D85" s="3">
-        <v>0</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -3103,7 +3103,7 @@
         <v>73253732352</v>
       </c>
       <c r="D86" s="3">
-        <v>0</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -3117,7 +3117,7 @@
         <v>29677795328</v>
       </c>
       <c r="D87" s="3">
-        <v>0</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3131,7 +3131,7 @@
         <v>13105030144</v>
       </c>
       <c r="D88" s="3">
-        <v>0</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3145,7 +3145,7 @@
         <v>33733912576</v>
       </c>
       <c r="D89" s="3">
-        <v>0</v>
+        <v>7817</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -3159,7 +3159,7 @@
         <v>69418459136</v>
       </c>
       <c r="D90" s="3">
-        <v>0</v>
+        <v>2569</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3173,7 +3173,7 @@
         <v>11092198400</v>
       </c>
       <c r="D91" s="3">
-        <v>0</v>
+        <v>3253</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3187,7 +3187,7 @@
         <v>196070703104</v>
       </c>
       <c r="D92" s="3">
-        <v>0</v>
+        <v>489</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3201,7 +3201,7 @@
         <v>22804768768</v>
       </c>
       <c r="D93" s="3">
-        <v>0</v>
+        <v>921</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -3215,7 +3215,7 @@
         <v>43059806208</v>
       </c>
       <c r="D94" s="3">
-        <v>0</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3229,7 +3229,7 @@
         <v>23554387968</v>
       </c>
       <c r="D95" s="3">
-        <v>0</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3243,7 +3243,7 @@
         <v>8002731520</v>
       </c>
       <c r="D96" s="3">
-        <v>0</v>
+        <v>2715</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3257,7 +3257,7 @@
         <v>48619585536</v>
       </c>
       <c r="D97" s="3">
-        <v>0</v>
+        <v>790</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3271,7 +3271,7 @@
         <v>30291900416</v>
       </c>
       <c r="D98" s="3">
-        <v>0</v>
+        <v>3313</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3285,7 +3285,7 @@
         <v>21285398528</v>
       </c>
       <c r="D99" s="3">
-        <v>0</v>
+        <v>6094</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3299,7 +3299,7 @@
         <v>15602633728</v>
       </c>
       <c r="D100" s="3">
-        <v>0</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3313,7 +3313,7 @@
         <v>10206264320</v>
       </c>
       <c r="D101" s="3">
-        <v>0</v>
+        <v>998</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3327,7 +3327,7 @@
         <v>151204184064</v>
       </c>
       <c r="D102" s="3">
-        <v>0</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3341,7 +3341,7 @@
         <v>56442068992</v>
       </c>
       <c r="D103" s="3">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3355,7 +3355,7 @@
         <v>289030471680</v>
       </c>
       <c r="D104" s="3">
-        <v>0</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3369,7 +3369,7 @@
         <v>84548780032</v>
       </c>
       <c r="D105" s="3">
-        <v>0</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3383,7 +3383,7 @@
         <v>117035548672</v>
       </c>
       <c r="D106" s="3">
-        <v>0</v>
+        <v>688</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3397,7 +3397,7 @@
         <v>27037904896</v>
       </c>
       <c r="D107" s="3">
-        <v>0</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3411,7 +3411,7 @@
         <v>93960077312</v>
       </c>
       <c r="D108" s="3">
-        <v>0</v>
+        <v>588</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3425,7 +3425,7 @@
         <v>25035452416</v>
       </c>
       <c r="D109" s="3">
-        <v>0</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3439,7 +3439,7 @@
         <v>91060879360</v>
       </c>
       <c r="D110" s="3">
-        <v>0</v>
+        <v>880</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3453,7 +3453,7 @@
         <v>236137775104</v>
       </c>
       <c r="D111" s="3">
-        <v>0</v>
+        <v>3357</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3467,7 +3467,7 @@
         <v>134033604608</v>
       </c>
       <c r="D112" s="3">
-        <v>0</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3481,7 +3481,7 @@
         <v>21224155136</v>
       </c>
       <c r="D113" s="3">
-        <v>0</v>
+        <v>4129</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3495,7 +3495,7 @@
         <v>20692469760</v>
       </c>
       <c r="D114" s="3">
-        <v>0</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3509,7 +3509,7 @@
         <v>85765447680</v>
       </c>
       <c r="D115" s="3">
-        <v>0</v>
+        <v>835</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3523,7 +3523,7 @@
         <v>21061343232</v>
       </c>
       <c r="D116" s="3">
-        <v>0</v>
+        <v>2851</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3537,7 +3537,7 @@
         <v>277551644672</v>
       </c>
       <c r="D117" s="3">
-        <v>0</v>
+        <v>3102</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3551,7 +3551,7 @@
         <v>40037818368</v>
       </c>
       <c r="D118" s="3">
-        <v>0</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3565,7 +3565,7 @@
         <v>79053971456</v>
       </c>
       <c r="D119" s="3">
-        <v>0</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3579,7 +3579,7 @@
         <v>164860542976</v>
       </c>
       <c r="D120" s="3">
-        <v>0</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3593,7 +3593,7 @@
         <v>13148870656</v>
       </c>
       <c r="D121" s="3">
-        <v>0</v>
+        <v>7216</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3607,7 +3607,7 @@
         <v>140144295936</v>
       </c>
       <c r="D122" s="3">
-        <v>0</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3621,7 +3621,7 @@
         <v>35188596736</v>
       </c>
       <c r="D123" s="3">
-        <v>0</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3635,7 +3635,7 @@
         <v>43741097984</v>
       </c>
       <c r="D124" s="3">
-        <v>0</v>
+        <v>825</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3649,7 +3649,7 @@
         <v>80243499008</v>
       </c>
       <c r="D125" s="3">
-        <v>0</v>
+        <v>774</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3663,7 +3663,7 @@
         <v>20803835904</v>
       </c>
       <c r="D126" s="3">
-        <v>0</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3677,7 +3677,7 @@
         <v>61193662464</v>
       </c>
       <c r="D127" s="3">
-        <v>0</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3691,7 +3691,7 @@
         <v>41671692288</v>
       </c>
       <c r="D128" s="3">
-        <v>0</v>
+        <v>4084</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3705,7 +3705,7 @@
         <v>26572437504</v>
       </c>
       <c r="D129" s="3">
-        <v>0</v>
+        <v>521</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3719,7 +3719,7 @@
         <v>42955804672</v>
       </c>
       <c r="D130" s="3">
-        <v>0</v>
+        <v>3194</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3733,7 +3733,7 @@
         <v>33604399104</v>
       </c>
       <c r="D131" s="3">
-        <v>0</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3747,7 +3747,7 @@
         <v>430614740992</v>
       </c>
       <c r="D132" s="3">
-        <v>0</v>
+        <v>204</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3761,7 +3761,7 @@
         <v>19682297856</v>
       </c>
       <c r="D133" s="3">
-        <v>0</v>
+        <v>7440</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3775,7 +3775,7 @@
         <v>85615460352</v>
       </c>
       <c r="D134" s="3">
-        <v>0</v>
+        <v>574</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3789,7 +3789,7 @@
         <v>46371643392</v>
       </c>
       <c r="D135" s="3">
-        <v>0</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3803,7 +3803,7 @@
         <v>70541500416</v>
       </c>
       <c r="D136" s="3">
-        <v>0</v>
+        <v>5439</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3817,7 +3817,7 @@
         <v>51448737792</v>
       </c>
       <c r="D137" s="3">
-        <v>0</v>
+        <v>530</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3831,7 +3831,7 @@
         <v>75454087168</v>
       </c>
       <c r="D138" s="3">
-        <v>0</v>
+        <v>3321</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3845,7 +3845,7 @@
         <v>173122093056</v>
       </c>
       <c r="D139" s="3">
-        <v>0</v>
+        <v>829</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3859,7 +3859,7 @@
         <v>20711725056</v>
       </c>
       <c r="D140" s="3">
-        <v>0</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3873,7 +3873,7 @@
         <v>13629927424</v>
       </c>
       <c r="D141" s="3">
-        <v>0</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3887,7 +3887,7 @@
         <v>12614422528</v>
       </c>
       <c r="D142" s="3">
-        <v>0</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3901,7 +3901,7 @@
         <v>29770635264</v>
       </c>
       <c r="D143" s="3">
-        <v>0</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3915,7 +3915,7 @@
         <v>127497732096</v>
       </c>
       <c r="D144" s="3">
-        <v>0</v>
+        <v>426</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3929,7 +3929,7 @@
         <v>87314300928</v>
       </c>
       <c r="D145" s="3">
-        <v>0</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3943,7 +3943,7 @@
         <v>41181835264</v>
       </c>
       <c r="D146" s="3">
-        <v>0</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3957,7 +3957,7 @@
         <v>24929353728</v>
       </c>
       <c r="D147" s="3">
-        <v>0</v>
+        <v>5238</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3971,7 +3971,7 @@
         <v>30505474048</v>
       </c>
       <c r="D148" s="3">
-        <v>0</v>
+        <v>2549</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3985,7 +3985,7 @@
         <v>51854323712</v>
       </c>
       <c r="D149" s="3">
-        <v>0</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3999,7 +3999,7 @@
         <v>66026000384</v>
       </c>
       <c r="D150" s="3">
-        <v>0</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -4013,7 +4013,7 @@
         <v>45835534336</v>
       </c>
       <c r="D151" s="3">
-        <v>0</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -4027,7 +4027,7 @@
         <v>16992831488</v>
       </c>
       <c r="D152" s="3">
-        <v>0</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -4041,7 +4041,7 @@
         <v>15371940864</v>
       </c>
       <c r="D153" s="3">
-        <v>0</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -4055,7 +4055,7 @@
         <v>50148589568</v>
       </c>
       <c r="D154" s="3">
-        <v>0</v>
+        <v>3383</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -4069,7 +4069,7 @@
         <v>16443793408</v>
       </c>
       <c r="D155" s="3">
-        <v>0</v>
+        <v>417</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -4083,7 +4083,7 @@
         <v>28331427840</v>
       </c>
       <c r="D156" s="3">
-        <v>0</v>
+        <v>965</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -4097,7 +4097,7 @@
         <v>31252092928</v>
       </c>
       <c r="D157" s="3">
-        <v>0</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -4111,7 +4111,7 @@
         <v>54415687680</v>
       </c>
       <c r="D158" s="3">
-        <v>0</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -4125,7 +4125,7 @@
         <v>26111299584</v>
       </c>
       <c r="D159" s="3">
-        <v>0</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4139,7 +4139,7 @@
         <v>90704863232</v>
       </c>
       <c r="D160" s="3">
-        <v>0</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -4153,7 +4153,7 @@
         <v>35066421248</v>
       </c>
       <c r="D161" s="3">
-        <v>0</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4167,7 +4167,7 @@
         <v>12138409984</v>
       </c>
       <c r="D162" s="3">
-        <v>0</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4181,7 +4181,7 @@
         <v>148365983744</v>
       </c>
       <c r="D163" s="3">
-        <v>0</v>
+        <v>529</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -4195,7 +4195,7 @@
         <v>30804508672</v>
       </c>
       <c r="D164" s="3">
-        <v>0</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -4209,7 +4209,7 @@
         <v>70442205184</v>
       </c>
       <c r="D165" s="3">
-        <v>0</v>
+        <v>799</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -4223,7 +4223,7 @@
         <v>34208634880</v>
       </c>
       <c r="D166" s="3">
-        <v>0</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4237,7 +4237,7 @@
         <v>42506903552</v>
       </c>
       <c r="D167" s="3">
-        <v>0</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4251,7 +4251,7 @@
         <v>42926219264</v>
       </c>
       <c r="D168" s="3">
-        <v>0</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4265,7 +4265,7 @@
         <v>94383382528</v>
       </c>
       <c r="D169" s="3">
-        <v>0</v>
+        <v>488</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4279,7 +4279,7 @@
         <v>75608522752</v>
       </c>
       <c r="D170" s="3">
-        <v>0</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4293,7 +4293,7 @@
         <v>9639884800</v>
       </c>
       <c r="D171" s="3">
-        <v>0</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -4307,7 +4307,7 @@
         <v>33533446144</v>
       </c>
       <c r="D172" s="3">
-        <v>0</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -4321,7 +4321,7 @@
         <v>74952081408</v>
       </c>
       <c r="D173" s="3">
-        <v>0</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -4335,7 +4335,7 @@
         <v>13941564416</v>
       </c>
       <c r="D174" s="3">
-        <v>0</v>
+        <v>815</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4349,7 +4349,7 @@
         <v>27113322496</v>
       </c>
       <c r="D175" s="3">
-        <v>0</v>
+        <v>4375</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4363,7 +4363,7 @@
         <v>32420884480</v>
       </c>
       <c r="D176" s="3">
-        <v>0</v>
+        <v>760</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4377,7 +4377,7 @@
         <v>94701240320</v>
       </c>
       <c r="D177" s="3">
-        <v>0</v>
+        <v>202</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4391,7 +4391,7 @@
         <v>30301935616</v>
       </c>
       <c r="D178" s="3">
-        <v>0</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -4405,7 +4405,7 @@
         <v>22909251584</v>
       </c>
       <c r="D179" s="3">
-        <v>0</v>
+        <v>451</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4419,7 +4419,7 @@
         <v>20835123200</v>
       </c>
       <c r="D180" s="3">
-        <v>0</v>
+        <v>640</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4433,7 +4433,7 @@
         <v>26550040576</v>
       </c>
       <c r="D181" s="3">
-        <v>0</v>
+        <v>2756</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4447,7 +4447,7 @@
         <v>16718679040</v>
       </c>
       <c r="D182" s="3">
-        <v>0</v>
+        <v>512</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4461,7 +4461,7 @@
         <v>14948465664</v>
       </c>
       <c r="D183" s="3">
-        <v>0</v>
+        <v>3076</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4475,7 +4475,7 @@
         <v>23665893376</v>
       </c>
       <c r="D184" s="3">
-        <v>0</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4489,7 +4489,7 @@
         <v>39751077888</v>
       </c>
       <c r="D185" s="3">
-        <v>0</v>
+        <v>5025</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4503,7 +4503,7 @@
         <v>23733823488</v>
       </c>
       <c r="D186" s="3">
-        <v>0</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4517,7 +4517,7 @@
         <v>17026680832</v>
       </c>
       <c r="D187" s="3">
-        <v>0</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4531,7 +4531,7 @@
         <v>37707108352</v>
       </c>
       <c r="D188" s="3">
-        <v>0</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4545,7 +4545,7 @@
         <v>518444810240</v>
       </c>
       <c r="D189" s="3">
-        <v>0</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4559,7 +4559,7 @@
         <v>14674240512</v>
       </c>
       <c r="D190" s="3">
-        <v>0</v>
+        <v>794</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4573,7 +4573,7 @@
         <v>18639964160</v>
       </c>
       <c r="D191" s="3">
-        <v>0</v>
+        <v>405</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4587,7 +4587,7 @@
         <v>57826992128</v>
       </c>
       <c r="D192" s="3">
-        <v>0</v>
+        <v>83</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -4601,7 +4601,7 @@
         <v>47956336640</v>
       </c>
       <c r="D193" s="3">
-        <v>0</v>
+        <v>2379</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -4615,7 +4615,7 @@
         <v>10059698176</v>
       </c>
       <c r="D194" s="3">
-        <v>0</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4629,7 +4629,7 @@
         <v>74125393920</v>
       </c>
       <c r="D195" s="3">
-        <v>0</v>
+        <v>656</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4643,7 +4643,7 @@
         <v>46056202240</v>
       </c>
       <c r="D196" s="3">
-        <v>0</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4657,7 +4657,7 @@
         <v>32293390336</v>
       </c>
       <c r="D197" s="3">
-        <v>0</v>
+        <v>4136</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4671,7 +4671,7 @@
         <v>21333448704</v>
       </c>
       <c r="D198" s="3">
-        <v>0</v>
+        <v>997</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4685,7 +4685,7 @@
         <v>24562626560</v>
       </c>
       <c r="D199" s="3">
-        <v>0</v>
+        <v>4672</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4699,7 +4699,7 @@
         <v>125708337152</v>
       </c>
       <c r="D200" s="3">
-        <v>0</v>
+        <v>899</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4713,7 +4713,7 @@
         <v>7427730944</v>
       </c>
       <c r="D201" s="3">
-        <v>0</v>
+        <v>3364</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -4727,7 +4727,7 @@
         <v>44114644992</v>
       </c>
       <c r="D202" s="3">
-        <v>1</v>
+        <v>17862</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -4741,7 +4741,7 @@
         <v>72851357696</v>
       </c>
       <c r="D203" s="3">
-        <v>0</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4755,7 +4755,7 @@
         <v>27547740160</v>
       </c>
       <c r="D204" s="3">
-        <v>0</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4769,7 +4769,7 @@
         <v>20780531712</v>
       </c>
       <c r="D205" s="3">
-        <v>0</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4783,7 +4783,7 @@
         <v>20780527616</v>
       </c>
       <c r="D206" s="3">
-        <v>0</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -4797,7 +4797,7 @@
         <v>11918684160</v>
       </c>
       <c r="D207" s="3">
-        <v>0</v>
+        <v>8734</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4811,7 +4811,7 @@
         <v>63512309760</v>
       </c>
       <c r="D208" s="3">
-        <v>0</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -4825,7 +4825,7 @@
         <v>40824512512</v>
       </c>
       <c r="D209" s="3">
-        <v>0</v>
+        <v>935</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4839,7 +4839,7 @@
         <v>40050442240</v>
       </c>
       <c r="D210" s="3">
-        <v>0</v>
+        <v>383</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4853,7 +4853,7 @@
         <v>197149966336</v>
       </c>
       <c r="D211" s="3">
-        <v>0</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4867,7 +4867,7 @@
         <v>38020972544</v>
       </c>
       <c r="D212" s="3">
-        <v>0</v>
+        <v>2388</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4881,7 +4881,7 @@
         <v>92434636800</v>
       </c>
       <c r="D213" s="3">
-        <v>0</v>
+        <v>595</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4895,7 +4895,7 @@
         <v>19009925120</v>
       </c>
       <c r="D214" s="3">
-        <v>0</v>
+        <v>6444</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4909,7 +4909,7 @@
         <v>11328284672</v>
       </c>
       <c r="D215" s="3">
-        <v>0</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4923,7 +4923,7 @@
         <v>78093942784</v>
       </c>
       <c r="D216" s="3">
-        <v>0</v>
+        <v>700</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4937,7 +4937,7 @@
         <v>36784836608</v>
       </c>
       <c r="D217" s="3">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -4951,7 +4951,7 @@
         <v>61126762496</v>
       </c>
       <c r="D218" s="3">
-        <v>0</v>
+        <v>3576</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4965,7 +4965,7 @@
         <v>17639548928</v>
       </c>
       <c r="D219" s="3">
-        <v>0</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4979,7 +4979,7 @@
         <v>115379675136</v>
       </c>
       <c r="D220" s="3">
-        <v>0</v>
+        <v>2147</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -4993,7 +4993,7 @@
         <v>30381549568</v>
       </c>
       <c r="D221" s="3">
-        <v>0</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -5007,7 +5007,7 @@
         <v>9376664576</v>
       </c>
       <c r="D222" s="3">
-        <v>0</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -5021,7 +5021,7 @@
         <v>27776366592</v>
       </c>
       <c r="D223" s="3">
-        <v>0</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -5035,7 +5035,7 @@
         <v>191036227584</v>
       </c>
       <c r="D224" s="3">
-        <v>0</v>
+        <v>326</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -5049,7 +5049,7 @@
         <v>28006629376</v>
       </c>
       <c r="D225" s="3">
-        <v>0</v>
+        <v>6240</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -5063,7 +5063,7 @@
         <v>35871125504</v>
       </c>
       <c r="D226" s="3">
-        <v>0</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -5077,7 +5077,7 @@
         <v>9088489472</v>
       </c>
       <c r="D227" s="3">
-        <v>0</v>
+        <v>3051</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -5091,7 +5091,7 @@
         <v>82883837952</v>
       </c>
       <c r="D228" s="3">
-        <v>0</v>
+        <v>607</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5105,7 +5105,7 @@
         <v>15555615744</v>
       </c>
       <c r="D229" s="3">
-        <v>0</v>
+        <v>9040</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5119,7 +5119,7 @@
         <v>9682719744</v>
       </c>
       <c r="D230" s="3">
-        <v>0</v>
+        <v>2580</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5133,7 +5133,7 @@
         <v>35227938816</v>
       </c>
       <c r="D231" s="3">
-        <v>0</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5147,7 +5147,7 @@
         <v>45348806656</v>
       </c>
       <c r="D232" s="3">
-        <v>0</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -5161,7 +5161,7 @@
         <v>27557775360</v>
       </c>
       <c r="D233" s="3">
-        <v>0</v>
+        <v>9368</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -5175,7 +5175,7 @@
         <v>61783605248</v>
       </c>
       <c r="D234" s="3">
-        <v>0</v>
+        <v>784</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5189,7 +5189,7 @@
         <v>18041808896</v>
       </c>
       <c r="D235" s="3">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5203,7 +5203,7 @@
         <v>426281861120</v>
       </c>
       <c r="D236" s="3">
-        <v>0</v>
+        <v>463</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5217,7 +5217,7 @@
         <v>151462019072</v>
       </c>
       <c r="D237" s="3">
-        <v>0</v>
+        <v>853</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5231,7 +5231,7 @@
         <v>17783445504</v>
       </c>
       <c r="D238" s="3">
-        <v>0</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -5245,7 +5245,7 @@
         <v>13058195456</v>
       </c>
       <c r="D239" s="3">
-        <v>1</v>
+        <v>10793</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5259,7 +5259,7 @@
         <v>48093175808</v>
       </c>
       <c r="D240" s="3">
-        <v>0</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5273,7 +5273,7 @@
         <v>34133544960</v>
       </c>
       <c r="D241" s="3">
-        <v>0</v>
+        <v>5611</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5287,7 +5287,7 @@
         <v>24693260288</v>
       </c>
       <c r="D242" s="3">
-        <v>0</v>
+        <v>432</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5301,7 +5301,7 @@
         <v>35723571200</v>
       </c>
       <c r="D243" s="3">
-        <v>0</v>
+        <v>670</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5315,7 +5315,7 @@
         <v>26165108736</v>
       </c>
       <c r="D244" s="3">
-        <v>1</v>
+        <v>11038</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5329,7 +5329,7 @@
         <v>7801214464</v>
       </c>
       <c r="D245" s="3">
-        <v>0</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5343,7 +5343,7 @@
         <v>210273517568</v>
       </c>
       <c r="D246" s="3">
-        <v>0</v>
+        <v>874</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5357,7 +5357,7 @@
         <v>17499652096</v>
       </c>
       <c r="D247" s="3">
-        <v>0</v>
+        <v>862</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5371,7 +5371,7 @@
         <v>34535673856</v>
       </c>
       <c r="D248" s="3">
-        <v>0</v>
+        <v>471</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5385,7 +5385,7 @@
         <v>81951653888</v>
       </c>
       <c r="D249" s="3">
-        <v>0</v>
+        <v>716</v>
       </c>
     </row>
     <row r="250" spans="1:4">
@@ -5399,7 +5399,7 @@
         <v>14535428096</v>
       </c>
       <c r="D250" s="3">
-        <v>0</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5413,7 +5413,7 @@
         <v>41981759488</v>
       </c>
       <c r="D251" s="3">
-        <v>0</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -5427,7 +5427,7 @@
         <v>18723047424</v>
       </c>
       <c r="D252" s="3">
-        <v>0</v>
+        <v>745</v>
       </c>
     </row>
     <row r="253" spans="1:4">
@@ -5441,7 +5441,7 @@
         <v>103727644672</v>
       </c>
       <c r="D253" s="3">
-        <v>0</v>
+        <v>8266</v>
       </c>
     </row>
     <row r="254" spans="1:4">
@@ -5455,7 +5455,7 @@
         <v>92551520256</v>
       </c>
       <c r="D254" s="3">
-        <v>0</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -5469,7 +5469,7 @@
         <v>23359107072</v>
       </c>
       <c r="D255" s="3">
-        <v>0</v>
+        <v>2176</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -5483,7 +5483,7 @@
         <v>20438013952</v>
       </c>
       <c r="D256" s="3">
-        <v>0</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="257" spans="1:4">
@@ -5497,7 +5497,7 @@
         <v>11477002240</v>
       </c>
       <c r="D257" s="3">
-        <v>0</v>
+        <v>6452</v>
       </c>
     </row>
     <row r="258" spans="1:4">
@@ -5511,7 +5511,7 @@
         <v>179631128576</v>
       </c>
       <c r="D258" s="3">
-        <v>0</v>
+        <v>309</v>
       </c>
     </row>
     <row r="259" spans="1:4">
@@ -5525,7 +5525,7 @@
         <v>193049018368</v>
       </c>
       <c r="D259" s="3">
-        <v>0</v>
+        <v>366</v>
       </c>
     </row>
     <row r="260" spans="1:4">
@@ -5539,7 +5539,7 @@
         <v>8130369536</v>
       </c>
       <c r="D260" s="3">
-        <v>1</v>
+        <v>10989</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -5553,7 +5553,7 @@
         <v>21202290688</v>
       </c>
       <c r="D261" s="3">
-        <v>0</v>
+        <v>5804</v>
       </c>
     </row>
     <row r="262" spans="1:4">
@@ -5567,7 +5567,7 @@
         <v>36559507456</v>
       </c>
       <c r="D262" s="3">
-        <v>0</v>
+        <v>989</v>
       </c>
     </row>
     <row r="263" spans="1:4">
@@ -5581,7 +5581,7 @@
         <v>36459524096</v>
       </c>
       <c r="D263" s="3">
-        <v>0</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -5595,7 +5595,7 @@
         <v>19188992000</v>
       </c>
       <c r="D264" s="3">
-        <v>0</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="265" spans="1:4">
@@ -5609,7 +5609,7 @@
         <v>15327464448</v>
       </c>
       <c r="D265" s="3">
-        <v>0</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="266" spans="1:4">
@@ -5623,7 +5623,7 @@
         <v>12853967872</v>
       </c>
       <c r="D266" s="3">
-        <v>0</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="267" spans="1:4">
@@ -5637,7 +5637,7 @@
         <v>17507858432</v>
       </c>
       <c r="D267" s="3">
-        <v>0</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="268" spans="1:4">
@@ -5651,7 +5651,7 @@
         <v>374144532480</v>
       </c>
       <c r="D268" s="3">
-        <v>0</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -5665,7 +5665,7 @@
         <v>55530835968</v>
       </c>
       <c r="D269" s="3">
-        <v>0</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -5679,7 +5679,7 @@
         <v>703244009472</v>
       </c>
       <c r="D270" s="3">
-        <v>0</v>
+        <v>796</v>
       </c>
     </row>
     <row r="271" spans="1:4">
@@ -5693,7 +5693,7 @@
         <v>11892715520</v>
       </c>
       <c r="D271" s="3">
-        <v>0</v>
+        <v>5534</v>
       </c>
     </row>
     <row r="272" spans="1:4">
@@ -5707,7 +5707,7 @@
         <v>28020498432</v>
       </c>
       <c r="D272" s="3">
-        <v>0</v>
+        <v>2445</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -5721,7 +5721,7 @@
         <v>46263459840</v>
       </c>
       <c r="D273" s="3">
-        <v>0</v>
+        <v>8256</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -5735,7 +5735,7 @@
         <v>44288094208</v>
       </c>
       <c r="D274" s="3">
-        <v>0</v>
+        <v>6089</v>
       </c>
     </row>
     <row r="275" spans="1:4">
@@ -5749,7 +5749,7 @@
         <v>19349833728</v>
       </c>
       <c r="D275" s="3">
-        <v>1</v>
+        <v>10205</v>
       </c>
     </row>
     <row r="276" spans="1:4">
@@ -5763,7 +5763,7 @@
         <v>29485787136</v>
       </c>
       <c r="D276" s="3">
-        <v>0</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="277" spans="1:4">
@@ -5777,7 +5777,7 @@
         <v>46471135232</v>
       </c>
       <c r="D277" s="3">
-        <v>0</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="278" spans="1:4">
@@ -5791,7 +5791,7 @@
         <v>17377806336</v>
       </c>
       <c r="D278" s="3">
-        <v>0</v>
+        <v>7775</v>
       </c>
     </row>
     <row r="279" spans="1:4">
@@ -5805,7 +5805,7 @@
         <v>62805762048</v>
       </c>
       <c r="D279" s="3">
-        <v>0</v>
+        <v>7032</v>
       </c>
     </row>
     <row r="280" spans="1:4">
@@ -5819,7 +5819,7 @@
         <v>147675201536</v>
       </c>
       <c r="D280" s="3">
-        <v>0</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5833,7 +5833,7 @@
         <v>86546735104</v>
       </c>
       <c r="D281" s="3">
-        <v>0</v>
+        <v>307</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -5847,7 +5847,7 @@
         <v>38657167360</v>
       </c>
       <c r="D282" s="3">
-        <v>0</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -5861,7 +5861,7 @@
         <v>44190527488</v>
       </c>
       <c r="D283" s="3">
-        <v>0</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -5875,7 +5875,7 @@
         <v>46705745920</v>
       </c>
       <c r="D284" s="3">
-        <v>0</v>
+        <v>807</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5889,7 +5889,7 @@
         <v>20253243392</v>
       </c>
       <c r="D285" s="3">
-        <v>0</v>
+        <v>824</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -5903,7 +5903,7 @@
         <v>95060656128</v>
       </c>
       <c r="D286" s="3">
-        <v>0</v>
+        <v>2690</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5917,7 +5917,7 @@
         <v>11014268928</v>
       </c>
       <c r="D287" s="3">
-        <v>0</v>
+        <v>2573</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5931,7 +5931,7 @@
         <v>38469877760</v>
       </c>
       <c r="D288" s="3">
-        <v>0</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5945,7 +5945,7 @@
         <v>22069817344</v>
       </c>
       <c r="D289" s="3">
-        <v>0</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -5959,7 +5959,7 @@
         <v>46908121088</v>
       </c>
       <c r="D290" s="3">
-        <v>0</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5973,7 +5973,7 @@
         <v>715270914048</v>
       </c>
       <c r="D291" s="3">
-        <v>0</v>
+        <v>249</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -5987,7 +5987,7 @@
         <v>219504082944</v>
       </c>
       <c r="D292" s="3">
-        <v>0</v>
+        <v>431</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -6001,7 +6001,7 @@
         <v>32221650944</v>
       </c>
       <c r="D293" s="3">
-        <v>0</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -6015,7 +6015,7 @@
         <v>10213828608</v>
       </c>
       <c r="D294" s="3">
-        <v>0</v>
+        <v>5059</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -6029,7 +6029,7 @@
         <v>125488693248</v>
       </c>
       <c r="D295" s="3">
-        <v>0</v>
+        <v>375</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -6043,7 +6043,7 @@
         <v>18853021696</v>
       </c>
       <c r="D296" s="3">
-        <v>0</v>
+        <v>2292</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -6057,7 +6057,7 @@
         <v>154256687104</v>
       </c>
       <c r="D297" s="3">
-        <v>0</v>
+        <v>729</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -6071,7 +6071,7 @@
         <v>39229546496</v>
       </c>
       <c r="D298" s="3">
-        <v>0</v>
+        <v>619</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -6085,7 +6085,7 @@
         <v>27065245696</v>
       </c>
       <c r="D299" s="3">
-        <v>0</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -6099,7 +6099,7 @@
         <v>36635373568</v>
       </c>
       <c r="D300" s="3">
-        <v>0</v>
+        <v>903</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -6113,7 +6113,7 @@
         <v>50184888320</v>
       </c>
       <c r="D301" s="3">
-        <v>0</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -6127,7 +6127,7 @@
         <v>9867600896</v>
       </c>
       <c r="D302" s="3">
-        <v>0</v>
+        <v>768</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -6141,7 +6141,7 @@
         <v>80336084992</v>
       </c>
       <c r="D303" s="3">
-        <v>0</v>
+        <v>687</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -6155,7 +6155,7 @@
         <v>114549284864</v>
       </c>
       <c r="D304" s="3">
-        <v>0</v>
+        <v>852</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -6169,7 +6169,7 @@
         <v>36670861312</v>
       </c>
       <c r="D305" s="3">
-        <v>0</v>
+        <v>331</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -6183,7 +6183,7 @@
         <v>17380739072</v>
       </c>
       <c r="D306" s="3">
-        <v>0</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -6197,7 +6197,7 @@
         <v>488635105280</v>
       </c>
       <c r="D307" s="3">
-        <v>0</v>
+        <v>373</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -6211,7 +6211,7 @@
         <v>8220720128</v>
       </c>
       <c r="D308" s="3">
-        <v>0</v>
+        <v>6072</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -6225,7 +6225,7 @@
         <v>20867567616</v>
       </c>
       <c r="D309" s="3">
-        <v>0</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -6239,7 +6239,7 @@
         <v>212126695424</v>
       </c>
       <c r="D310" s="3">
-        <v>0</v>
+        <v>671</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -6253,7 +6253,7 @@
         <v>79781789696</v>
       </c>
       <c r="D311" s="3">
-        <v>0</v>
+        <v>316</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -6267,7 +6267,7 @@
         <v>110969380864</v>
       </c>
       <c r="D312" s="3">
-        <v>0</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -6281,7 +6281,7 @@
         <v>260856004608</v>
       </c>
       <c r="D313" s="3">
-        <v>0</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="314" spans="1:4">
@@ -6295,7 +6295,7 @@
         <v>1436937093120</v>
       </c>
       <c r="D314" s="3">
-        <v>0</v>
+        <v>346</v>
       </c>
     </row>
     <row r="315" spans="1:4">
@@ -6309,7 +6309,7 @@
         <v>61106073600</v>
       </c>
       <c r="D315" s="3">
-        <v>0</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="316" spans="1:4">
@@ -6323,7 +6323,7 @@
         <v>26403696640</v>
       </c>
       <c r="D316" s="3">
-        <v>0</v>
+        <v>158</v>
       </c>
     </row>
     <row r="317" spans="1:4">
@@ -6337,7 +6337,7 @@
         <v>11415351296</v>
       </c>
       <c r="D317" s="3">
-        <v>0</v>
+        <v>5185</v>
       </c>
     </row>
     <row r="318" spans="1:4">
@@ -6351,7 +6351,7 @@
         <v>36607971328</v>
       </c>
       <c r="D318" s="3">
-        <v>0</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="319" spans="1:4">
@@ -6365,7 +6365,7 @@
         <v>109399367680</v>
       </c>
       <c r="D319" s="3">
-        <v>0</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="320" spans="1:4">
@@ -6379,7 +6379,7 @@
         <v>3148374343680</v>
       </c>
       <c r="D320" s="3">
-        <v>0</v>
+        <v>469</v>
       </c>
     </row>
     <row r="321" spans="1:4">
@@ -6393,7 +6393,7 @@
         <v>19816738816</v>
       </c>
       <c r="D321" s="3">
-        <v>0</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="322" spans="1:4">
@@ -6407,7 +6407,7 @@
         <v>16697247744</v>
       </c>
       <c r="D322" s="3">
-        <v>0</v>
+        <v>4616</v>
       </c>
     </row>
     <row r="323" spans="1:4">
@@ -6421,7 +6421,7 @@
         <v>8763129856</v>
       </c>
       <c r="D323" s="3">
-        <v>0</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="324" spans="1:4">
@@ -6435,7 +6435,7 @@
         <v>17039879168</v>
       </c>
       <c r="D324" s="3">
-        <v>0</v>
+        <v>667</v>
       </c>
     </row>
     <row r="325" spans="1:4">
@@ -6449,7 +6449,7 @@
         <v>12615121920</v>
       </c>
       <c r="D325" s="3">
-        <v>0</v>
+        <v>3203</v>
       </c>
     </row>
     <row r="326" spans="1:4">
@@ -6463,7 +6463,7 @@
         <v>86997917696</v>
       </c>
       <c r="D326" s="3">
-        <v>0</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="327" spans="1:4">
@@ -6477,7 +6477,7 @@
         <v>27689480192</v>
       </c>
       <c r="D327" s="3">
-        <v>0</v>
+        <v>350</v>
       </c>
     </row>
     <row r="328" spans="1:4">
@@ -6491,7 +6491,7 @@
         <v>53624729600</v>
       </c>
       <c r="D328" s="3">
-        <v>0</v>
+        <v>3606</v>
       </c>
     </row>
     <row r="329" spans="1:4">
@@ -6505,7 +6505,7 @@
         <v>90774863872</v>
       </c>
       <c r="D329" s="3">
-        <v>0</v>
+        <v>397</v>
       </c>
     </row>
     <row r="330" spans="1:4">
@@ -6519,7 +6519,7 @@
         <v>212028981248</v>
       </c>
       <c r="D330" s="3">
-        <v>0</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="331" spans="1:4">
@@ -6533,7 +6533,7 @@
         <v>8404886016</v>
       </c>
       <c r="D331" s="3">
-        <v>0</v>
+        <v>7513</v>
       </c>
     </row>
     <row r="332" spans="1:4">
@@ -6547,7 +6547,7 @@
         <v>83670769664</v>
       </c>
       <c r="D332" s="3">
-        <v>0</v>
+        <v>397</v>
       </c>
     </row>
     <row r="333" spans="1:4">
@@ -6561,7 +6561,7 @@
         <v>47777492992</v>
       </c>
       <c r="D333" s="3">
-        <v>0</v>
+        <v>326</v>
       </c>
     </row>
     <row r="334" spans="1:4">
@@ -6575,7 +6575,7 @@
         <v>47733604352</v>
       </c>
       <c r="D334" s="3">
-        <v>0</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="335" spans="1:4">
@@ -6589,7 +6589,7 @@
         <v>24933447680</v>
       </c>
       <c r="D335" s="3">
-        <v>0</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="336" spans="1:4">
@@ -6603,7 +6603,7 @@
         <v>379074019328</v>
       </c>
       <c r="D336" s="3">
-        <v>0</v>
+        <v>224</v>
       </c>
     </row>
     <row r="337" spans="1:4">
@@ -6617,7 +6617,7 @@
         <v>47860244480</v>
       </c>
       <c r="D337" s="3">
-        <v>0</v>
+        <v>4740</v>
       </c>
     </row>
     <row r="338" spans="1:4">
@@ -6631,7 +6631,7 @@
         <v>17017422848</v>
       </c>
       <c r="D338" s="3">
-        <v>0</v>
+        <v>6773</v>
       </c>
     </row>
     <row r="339" spans="1:4">
@@ -6645,7 +6645,7 @@
         <v>17017423872</v>
       </c>
       <c r="D339" s="3">
-        <v>0</v>
+        <v>6195</v>
       </c>
     </row>
     <row r="340" spans="1:4">
@@ -6659,7 +6659,7 @@
         <v>161776992256</v>
       </c>
       <c r="D340" s="3">
-        <v>0</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="341" spans="1:4">
@@ -6673,7 +6673,7 @@
         <v>116608745472</v>
       </c>
       <c r="D341" s="3">
-        <v>0</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="342" spans="1:4">
@@ -6687,7 +6687,7 @@
         <v>17779611648</v>
       </c>
       <c r="D342" s="3">
-        <v>0</v>
+        <v>5219</v>
       </c>
     </row>
     <row r="343" spans="1:4">
@@ -6701,7 +6701,7 @@
         <v>14923799552</v>
       </c>
       <c r="D343" s="3">
-        <v>0</v>
+        <v>761</v>
       </c>
     </row>
     <row r="344" spans="1:4">
@@ -6715,7 +6715,7 @@
         <v>62408306688</v>
       </c>
       <c r="D344" s="3">
-        <v>0</v>
+        <v>720</v>
       </c>
     </row>
     <row r="345" spans="1:4">
@@ -6729,7 +6729,7 @@
         <v>22033913856</v>
       </c>
       <c r="D345" s="3">
-        <v>0</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="346" spans="1:4">
@@ -6743,7 +6743,7 @@
         <v>71339556864</v>
       </c>
       <c r="D346" s="3">
-        <v>0</v>
+        <v>406</v>
       </c>
     </row>
     <row r="347" spans="1:4">
@@ -6757,7 +6757,7 @@
         <v>11836951552</v>
       </c>
       <c r="D347" s="3">
-        <v>0</v>
+        <v>7393</v>
       </c>
     </row>
     <row r="348" spans="1:4">
@@ -6771,7 +6771,7 @@
         <v>20582731776</v>
       </c>
       <c r="D348" s="3">
-        <v>0</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="349" spans="1:4">
@@ -6785,7 +6785,7 @@
         <v>36341940224</v>
       </c>
       <c r="D349" s="3">
-        <v>0</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="350" spans="1:4">
@@ -6799,7 +6799,7 @@
         <v>3385742589952</v>
       </c>
       <c r="D350" s="3">
-        <v>0</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="351" spans="1:4">
@@ -6813,7 +6813,7 @@
         <v>28296708096</v>
       </c>
       <c r="D351" s="3">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="352" spans="1:4">
@@ -6827,7 +6827,7 @@
         <v>58295758848</v>
       </c>
       <c r="D352" s="3">
-        <v>0</v>
+        <v>866</v>
       </c>
     </row>
     <row r="353" spans="1:4">
@@ -6841,7 +6841,7 @@
         <v>71771955200</v>
       </c>
       <c r="D353" s="3">
-        <v>0</v>
+        <v>159</v>
       </c>
     </row>
     <row r="354" spans="1:4">
@@ -6855,7 +6855,7 @@
         <v>47461388288</v>
       </c>
       <c r="D354" s="3">
-        <v>0</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="355" spans="1:4">
@@ -6869,7 +6869,7 @@
         <v>48066940928</v>
       </c>
       <c r="D355" s="3">
-        <v>0</v>
+        <v>883</v>
       </c>
     </row>
     <row r="356" spans="1:4">
@@ -6883,7 +6883,7 @@
         <v>20449646592</v>
       </c>
       <c r="D356" s="3">
-        <v>0</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="357" spans="1:4">
@@ -6897,7 +6897,7 @@
         <v>30282682368</v>
       </c>
       <c r="D357" s="3">
-        <v>0</v>
+        <v>2795</v>
       </c>
     </row>
     <row r="358" spans="1:4">
@@ -6911,7 +6911,7 @@
         <v>66370912256</v>
       </c>
       <c r="D358" s="3">
-        <v>0</v>
+        <v>1750</v>
       </c>
     </row>
     <row r="359" spans="1:4">
@@ -6925,7 +6925,7 @@
         <v>512202702848</v>
       </c>
       <c r="D359" s="3">
-        <v>0</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="360" spans="1:4">
@@ -6939,7 +6939,7 @@
         <v>41136492544</v>
       </c>
       <c r="D360" s="3">
-        <v>0</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="361" spans="1:4">
@@ -6953,7 +6953,7 @@
         <v>61343215616</v>
       </c>
       <c r="D361" s="3">
-        <v>0</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="362" spans="1:4">
@@ -6967,7 +6967,7 @@
         <v>22347948032</v>
       </c>
       <c r="D362" s="3">
-        <v>0</v>
+        <v>798</v>
       </c>
     </row>
     <row r="363" spans="1:4">
@@ -6981,7 +6981,7 @@
         <v>150463119360</v>
       </c>
       <c r="D363" s="3">
-        <v>0</v>
+        <v>2963</v>
       </c>
     </row>
     <row r="364" spans="1:4">
@@ -6995,7 +6995,7 @@
         <v>127243747328</v>
       </c>
       <c r="D364" s="3">
-        <v>0</v>
+        <v>512</v>
       </c>
     </row>
     <row r="365" spans="1:4">
@@ -7009,7 +7009,7 @@
         <v>7678675456</v>
       </c>
       <c r="D365" s="3">
-        <v>1</v>
+        <v>18323</v>
       </c>
     </row>
     <row r="366" spans="1:4">
@@ -7023,7 +7023,7 @@
         <v>90477289472</v>
       </c>
       <c r="D366" s="3">
-        <v>0</v>
+        <v>282</v>
       </c>
     </row>
     <row r="367" spans="1:4">
@@ -7037,7 +7037,7 @@
         <v>52642279424</v>
       </c>
       <c r="D367" s="3">
-        <v>0</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="368" spans="1:4">
@@ -7051,7 +7051,7 @@
         <v>13372971008</v>
       </c>
       <c r="D368" s="3">
-        <v>0</v>
+        <v>857</v>
       </c>
     </row>
     <row r="369" spans="1:4">
@@ -7065,7 +7065,7 @@
         <v>86990397440</v>
       </c>
       <c r="D369" s="3">
-        <v>0</v>
+        <v>2291</v>
       </c>
     </row>
     <row r="370" spans="1:4">
@@ -7079,7 +7079,7 @@
         <v>18008526848</v>
       </c>
       <c r="D370" s="3">
-        <v>0</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="371" spans="1:4">
@@ -7093,7 +7093,7 @@
         <v>224251756544</v>
       </c>
       <c r="D371" s="3">
-        <v>0</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="372" spans="1:4">
@@ -7107,7 +7107,7 @@
         <v>148531806208</v>
       </c>
       <c r="D372" s="3">
-        <v>0</v>
+        <v>7585</v>
       </c>
     </row>
     <row r="373" spans="1:4">
@@ -7121,7 +7121,7 @@
         <v>56568721408</v>
       </c>
       <c r="D373" s="3">
-        <v>0</v>
+        <v>9191</v>
       </c>
     </row>
     <row r="374" spans="1:4">
@@ -7135,7 +7135,7 @@
         <v>206885666816</v>
       </c>
       <c r="D374" s="3">
-        <v>0</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="375" spans="1:4">
@@ -7149,7 +7149,7 @@
         <v>55332261888</v>
       </c>
       <c r="D375" s="3">
-        <v>0</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="376" spans="1:4">
@@ -7163,7 +7163,7 @@
         <v>10746920960</v>
       </c>
       <c r="D376" s="3">
-        <v>0</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="377" spans="1:4">
@@ -7177,7 +7177,7 @@
         <v>85308473344</v>
       </c>
       <c r="D377" s="3">
-        <v>0</v>
+        <v>925</v>
       </c>
     </row>
     <row r="378" spans="1:4">
@@ -7191,7 +7191,7 @@
         <v>14350348288</v>
       </c>
       <c r="D378" s="3">
-        <v>0</v>
+        <v>527</v>
       </c>
     </row>
     <row r="379" spans="1:4">
@@ -7205,7 +7205,7 @@
         <v>28853839872</v>
       </c>
       <c r="D379" s="3">
-        <v>0</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="380" spans="1:4">
@@ -7219,7 +7219,7 @@
         <v>25828954112</v>
       </c>
       <c r="D380" s="3">
-        <v>0</v>
+        <v>5691</v>
       </c>
     </row>
     <row r="381" spans="1:4">
@@ -7233,7 +7233,7 @@
         <v>19963203584</v>
       </c>
       <c r="D381" s="3">
-        <v>0</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="382" spans="1:4">
@@ -7247,7 +7247,7 @@
         <v>422401081344</v>
       </c>
       <c r="D382" s="3">
-        <v>0</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="383" spans="1:4">
@@ -7261,7 +7261,7 @@
         <v>157513121792</v>
       </c>
       <c r="D383" s="3">
-        <v>0</v>
+        <v>739</v>
       </c>
     </row>
     <row r="384" spans="1:4">
@@ -7275,7 +7275,7 @@
         <v>108158713856</v>
       </c>
       <c r="D384" s="3">
-        <v>0</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="385" spans="1:4">
@@ -7289,7 +7289,7 @@
         <v>46100111360</v>
       </c>
       <c r="D385" s="3">
-        <v>0</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="386" spans="1:4">
@@ -7303,7 +7303,7 @@
         <v>46982619136</v>
       </c>
       <c r="D386" s="3">
-        <v>0</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="387" spans="1:4">
@@ -7317,7 +7317,7 @@
         <v>24033007616</v>
       </c>
       <c r="D387" s="3">
-        <v>0</v>
+        <v>993</v>
       </c>
     </row>
     <row r="388" spans="1:4">
@@ -7331,7 +7331,7 @@
         <v>61526188032</v>
       </c>
       <c r="D388" s="3">
-        <v>0</v>
+        <v>571</v>
       </c>
     </row>
     <row r="389" spans="1:4">
@@ -7345,7 +7345,7 @@
         <v>27999809536</v>
       </c>
       <c r="D389" s="3">
-        <v>0</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="390" spans="1:4">
@@ -7359,7 +7359,7 @@
         <v>6527069184</v>
       </c>
       <c r="D390" s="3">
-        <v>0</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="391" spans="1:4">
@@ -7373,7 +7373,7 @@
         <v>50855284736</v>
       </c>
       <c r="D391" s="3">
-        <v>0</v>
+        <v>577</v>
       </c>
     </row>
     <row r="392" spans="1:4">
@@ -7387,7 +7387,7 @@
         <v>176126836736</v>
       </c>
       <c r="D392" s="3">
-        <v>0</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="393" spans="1:4">
@@ -7401,7 +7401,7 @@
         <v>18228981760</v>
       </c>
       <c r="D393" s="3">
-        <v>0</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="394" spans="1:4">
@@ -7415,7 +7415,7 @@
         <v>13827445760</v>
       </c>
       <c r="D394" s="3">
-        <v>0</v>
+        <v>859</v>
       </c>
     </row>
     <row r="395" spans="1:4">
@@ -7429,7 +7429,7 @@
         <v>34707984384</v>
       </c>
       <c r="D395" s="3">
-        <v>0</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="396" spans="1:4">
@@ -7443,7 +7443,7 @@
         <v>162158166016</v>
       </c>
       <c r="D396" s="3">
-        <v>0</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="397" spans="1:4">
@@ -7457,7 +7457,7 @@
         <v>51042308096</v>
       </c>
       <c r="D397" s="3">
-        <v>0</v>
+        <v>3434</v>
       </c>
     </row>
     <row r="398" spans="1:4">
@@ -7471,7 +7471,7 @@
         <v>13861316608</v>
       </c>
       <c r="D398" s="3">
-        <v>0</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="399" spans="1:4">
@@ -7485,7 +7485,7 @@
         <v>82952568832</v>
       </c>
       <c r="D399" s="3">
-        <v>0</v>
+        <v>264</v>
       </c>
     </row>
     <row r="400" spans="1:4">
@@ -7499,7 +7499,7 @@
         <v>24775632896</v>
       </c>
       <c r="D400" s="3">
-        <v>0</v>
+        <v>7292</v>
       </c>
     </row>
     <row r="401" spans="1:4">
@@ -7513,7 +7513,7 @@
         <v>68361080832</v>
       </c>
       <c r="D401" s="3">
-        <v>0</v>
+        <v>910</v>
       </c>
     </row>
     <row r="402" spans="1:4">
@@ -7527,7 +7527,7 @@
         <v>36600463360</v>
       </c>
       <c r="D402" s="3">
-        <v>0</v>
+        <v>798</v>
       </c>
     </row>
     <row r="403" spans="1:4">
@@ -7541,7 +7541,7 @@
         <v>14145387520</v>
       </c>
       <c r="D403" s="3">
-        <v>0</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="404" spans="1:4">
@@ -7555,7 +7555,7 @@
         <v>33320421376</v>
       </c>
       <c r="D404" s="3">
-        <v>0</v>
+        <v>673</v>
       </c>
     </row>
     <row r="405" spans="1:4">
@@ -7569,7 +7569,7 @@
         <v>24777056256</v>
       </c>
       <c r="D405" s="3">
-        <v>0</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="406" spans="1:4">
@@ -7583,7 +7583,7 @@
         <v>60738793472</v>
       </c>
       <c r="D406" s="3">
-        <v>0</v>
+        <v>350</v>
       </c>
     </row>
     <row r="407" spans="1:4">
@@ -7597,7 +7597,7 @@
         <v>51379978240</v>
       </c>
       <c r="D407" s="3">
-        <v>0</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="408" spans="1:4">
@@ -7611,7 +7611,7 @@
         <v>65621635072</v>
       </c>
       <c r="D408" s="3">
-        <v>0</v>
+        <v>814</v>
       </c>
     </row>
     <row r="409" spans="1:4">
@@ -7625,7 +7625,7 @@
         <v>162243543040</v>
       </c>
       <c r="D409" s="3">
-        <v>0</v>
+        <v>380</v>
       </c>
     </row>
     <row r="410" spans="1:4">
@@ -7639,7 +7639,7 @@
         <v>315489550336</v>
       </c>
       <c r="D410" s="3">
-        <v>0</v>
+        <v>602</v>
       </c>
     </row>
     <row r="411" spans="1:4">
@@ -7653,7 +7653,7 @@
         <v>24570071040</v>
       </c>
       <c r="D411" s="3">
-        <v>0</v>
+        <v>878</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -7667,7 +7667,7 @@
         <v>62049869824</v>
       </c>
       <c r="D412" s="3">
-        <v>0</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="413" spans="1:4">
@@ -7681,7 +7681,7 @@
         <v>21434335232</v>
       </c>
       <c r="D413" s="3">
-        <v>0</v>
+        <v>1961</v>
       </c>
     </row>
     <row r="414" spans="1:4">
@@ -7695,7 +7695,7 @@
         <v>59716870144</v>
       </c>
       <c r="D414" s="3">
-        <v>0</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="415" spans="1:4">
@@ -7709,7 +7709,7 @@
         <v>216517296128</v>
       </c>
       <c r="D415" s="3">
-        <v>0</v>
+        <v>189</v>
       </c>
     </row>
     <row r="416" spans="1:4">
@@ -7723,7 +7723,7 @@
         <v>100086374400</v>
       </c>
       <c r="D416" s="3">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="417" spans="1:4">
@@ -7737,7 +7737,7 @@
         <v>68993212416</v>
       </c>
       <c r="D417" s="3">
-        <v>0</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="418" spans="1:4">
@@ -7751,7 +7751,7 @@
         <v>14007479296</v>
       </c>
       <c r="D418" s="3">
-        <v>0</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="419" spans="1:4">
@@ -7765,7 +7765,7 @@
         <v>12557120512</v>
       </c>
       <c r="D419" s="3">
-        <v>0</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="420" spans="1:4">
@@ -7779,7 +7779,7 @@
         <v>28618983424</v>
       </c>
       <c r="D420" s="3">
-        <v>0</v>
+        <v>3613</v>
       </c>
     </row>
     <row r="421" spans="1:4">
@@ -7793,7 +7793,7 @@
         <v>19411460096</v>
       </c>
       <c r="D421" s="3">
-        <v>0</v>
+        <v>537</v>
       </c>
     </row>
     <row r="422" spans="1:4">
@@ -7807,7 +7807,7 @@
         <v>12521472000</v>
       </c>
       <c r="D422" s="3">
-        <v>0</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="423" spans="1:4">
@@ -7821,7 +7821,7 @@
         <v>98326429696</v>
       </c>
       <c r="D423" s="3">
-        <v>0</v>
+        <v>2230</v>
       </c>
     </row>
     <row r="424" spans="1:4">
@@ -7835,7 +7835,7 @@
         <v>19407491072</v>
       </c>
       <c r="D424" s="3">
-        <v>0</v>
+        <v>6143</v>
       </c>
     </row>
     <row r="425" spans="1:4">
@@ -7849,7 +7849,7 @@
         <v>13839256576</v>
       </c>
       <c r="D425" s="3">
-        <v>0</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="426" spans="1:4">
@@ -7863,7 +7863,7 @@
         <v>116169138176</v>
       </c>
       <c r="D426" s="3">
-        <v>0</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="427" spans="1:4">
@@ -7877,7 +7877,7 @@
         <v>28960364544</v>
       </c>
       <c r="D427" s="3">
-        <v>0</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="428" spans="1:4">
@@ -7891,7 +7891,7 @@
         <v>22116630528</v>
       </c>
       <c r="D428" s="3">
-        <v>0</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="429" spans="1:4">
@@ -7905,7 +7905,7 @@
         <v>21622820864</v>
       </c>
       <c r="D429" s="3">
-        <v>0</v>
+        <v>907</v>
       </c>
     </row>
     <row r="430" spans="1:4">
@@ -7919,7 +7919,7 @@
         <v>149493858304</v>
       </c>
       <c r="D430" s="3">
-        <v>0</v>
+        <v>506</v>
       </c>
     </row>
     <row r="431" spans="1:4">
@@ -7933,7 +7933,7 @@
         <v>20535781376</v>
       </c>
       <c r="D431" s="3">
-        <v>0</v>
+        <v>6090</v>
       </c>
     </row>
     <row r="432" spans="1:4">
@@ -7947,7 +7947,7 @@
         <v>26288504832</v>
       </c>
       <c r="D432" s="3">
-        <v>0</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="433" spans="1:4">
@@ -7961,7 +7961,7 @@
         <v>85791883264</v>
       </c>
       <c r="D433" s="3">
-        <v>0</v>
+        <v>355</v>
       </c>
     </row>
     <row r="434" spans="1:4">
@@ -7975,7 +7975,7 @@
         <v>37878435840</v>
       </c>
       <c r="D434" s="3">
-        <v>0</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="435" spans="1:4">
@@ -7989,7 +7989,7 @@
         <v>286571397120</v>
       </c>
       <c r="D435" s="3">
-        <v>0</v>
+        <v>805</v>
       </c>
     </row>
     <row r="436" spans="1:4">
@@ -8003,7 +8003,7 @@
         <v>27583377408</v>
       </c>
       <c r="D436" s="3">
-        <v>0</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="437" spans="1:4">
@@ -8017,7 +8017,7 @@
         <v>33084616704</v>
       </c>
       <c r="D437" s="3">
-        <v>0</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="438" spans="1:4">
@@ -8031,7 +8031,7 @@
         <v>14513481728</v>
       </c>
       <c r="D438" s="3">
-        <v>0</v>
+        <v>3192</v>
       </c>
     </row>
     <row r="439" spans="1:4">
@@ -8045,7 +8045,7 @@
         <v>44550275072</v>
       </c>
       <c r="D439" s="3">
-        <v>0</v>
+        <v>973</v>
       </c>
     </row>
     <row r="440" spans="1:4">
@@ -8059,7 +8059,7 @@
         <v>60626030592</v>
       </c>
       <c r="D440" s="3">
-        <v>0</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="441" spans="1:4">
@@ -8073,7 +8073,7 @@
         <v>45218430976</v>
       </c>
       <c r="D441" s="3">
-        <v>0</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="442" spans="1:4">
@@ -8087,7 +8087,7 @@
         <v>22633836544</v>
       </c>
       <c r="D442" s="3">
-        <v>0</v>
+        <v>409</v>
       </c>
     </row>
     <row r="443" spans="1:4">
@@ -8101,7 +8101,7 @@
         <v>8956667904</v>
       </c>
       <c r="D443" s="3">
-        <v>0</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="444" spans="1:4">
@@ -8115,7 +8115,7 @@
         <v>17914710016</v>
       </c>
       <c r="D444" s="3">
-        <v>0</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="445" spans="1:4">
@@ -8129,7 +8129,7 @@
         <v>1107984384000</v>
       </c>
       <c r="D445" s="3">
-        <v>0</v>
+        <v>575</v>
       </c>
     </row>
     <row r="446" spans="1:4">
@@ -8143,7 +8143,7 @@
         <v>183382982656</v>
       </c>
       <c r="D446" s="3">
-        <v>0</v>
+        <v>988</v>
       </c>
     </row>
     <row r="447" spans="1:4">
@@ -8157,7 +8157,7 @@
         <v>37602754560</v>
       </c>
       <c r="D447" s="3">
-        <v>0</v>
+        <v>124</v>
       </c>
     </row>
     <row r="448" spans="1:4">
@@ -8171,7 +8171,7 @@
         <v>15885391872</v>
       </c>
       <c r="D448" s="3">
-        <v>0</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="449" spans="1:4">
@@ -8185,7 +8185,7 @@
         <v>202583474176</v>
       </c>
       <c r="D449" s="3">
-        <v>0</v>
+        <v>375</v>
       </c>
     </row>
     <row r="450" spans="1:4">
@@ -8199,7 +8199,7 @@
         <v>142518648832</v>
       </c>
       <c r="D450" s="3">
-        <v>0</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="451" spans="1:4">
@@ -8213,7 +8213,7 @@
         <v>30307020800</v>
       </c>
       <c r="D451" s="3">
-        <v>0</v>
+        <v>700</v>
       </c>
     </row>
     <row r="452" spans="1:4">
@@ -8227,7 +8227,7 @@
         <v>93659488256</v>
       </c>
       <c r="D452" s="3">
-        <v>0</v>
+        <v>477</v>
       </c>
     </row>
     <row r="453" spans="1:4">
@@ -8241,7 +8241,7 @@
         <v>70455001088</v>
       </c>
       <c r="D453" s="3">
-        <v>0</v>
+        <v>158</v>
       </c>
     </row>
     <row r="454" spans="1:4">
@@ -8255,7 +8255,7 @@
         <v>60536872960</v>
       </c>
       <c r="D454" s="3">
-        <v>0</v>
+        <v>747</v>
       </c>
     </row>
     <row r="455" spans="1:4">
@@ -8269,7 +8269,7 @@
         <v>17819858944</v>
       </c>
       <c r="D455" s="3">
-        <v>0</v>
+        <v>2724</v>
       </c>
     </row>
     <row r="456" spans="1:4">
@@ -8283,7 +8283,7 @@
         <v>63389126656</v>
       </c>
       <c r="D456" s="3">
-        <v>0</v>
+        <v>4169</v>
       </c>
     </row>
     <row r="457" spans="1:4">
@@ -8297,7 +8297,7 @@
         <v>26981955584</v>
       </c>
       <c r="D457" s="3">
-        <v>0</v>
+        <v>315</v>
       </c>
     </row>
     <row r="458" spans="1:4">
@@ -8311,7 +8311,7 @@
         <v>22935490560</v>
       </c>
       <c r="D458" s="3">
-        <v>0</v>
+        <v>3082</v>
       </c>
     </row>
     <row r="459" spans="1:4">
@@ -8325,7 +8325,7 @@
         <v>83430293504</v>
       </c>
       <c r="D459" s="3">
-        <v>0</v>
+        <v>3730</v>
       </c>
     </row>
     <row r="460" spans="1:4">
@@ -8339,7 +8339,7 @@
         <v>151526883328</v>
       </c>
       <c r="D460" s="3">
-        <v>0</v>
+        <v>2762</v>
       </c>
     </row>
     <row r="461" spans="1:4">
@@ -8353,7 +8353,7 @@
         <v>17404329984</v>
       </c>
       <c r="D461" s="3">
-        <v>0</v>
+        <v>4335</v>
       </c>
     </row>
     <row r="462" spans="1:4">
@@ -8367,7 +8367,7 @@
         <v>18216427520</v>
       </c>
       <c r="D462" s="3">
-        <v>0</v>
+        <v>514</v>
       </c>
     </row>
     <row r="463" spans="1:4">
@@ -8381,7 +8381,7 @@
         <v>148672299008</v>
       </c>
       <c r="D463" s="3">
-        <v>0</v>
+        <v>812</v>
       </c>
     </row>
     <row r="464" spans="1:4">
@@ -8395,7 +8395,7 @@
         <v>31845064704</v>
       </c>
       <c r="D464" s="3">
-        <v>0</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="465" spans="1:4">
@@ -8409,7 +8409,7 @@
         <v>115785179136</v>
       </c>
       <c r="D465" s="3">
-        <v>0</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="466" spans="1:4">
@@ -8423,7 +8423,7 @@
         <v>56828997632</v>
       </c>
       <c r="D466" s="3">
-        <v>0</v>
+        <v>229</v>
       </c>
     </row>
     <row r="467" spans="1:4">
@@ -8437,7 +8437,7 @@
         <v>561557340160</v>
       </c>
       <c r="D467" s="3">
-        <v>0</v>
+        <v>325</v>
       </c>
     </row>
     <row r="468" spans="1:4">
@@ -8451,7 +8451,7 @@
         <v>13522948096</v>
       </c>
       <c r="D468" s="3">
-        <v>0</v>
+        <v>969</v>
       </c>
     </row>
     <row r="469" spans="1:4">
@@ -8465,7 +8465,7 @@
         <v>44030640128</v>
       </c>
       <c r="D469" s="3">
-        <v>0</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="470" spans="1:4">
@@ -8479,7 +8479,7 @@
         <v>27075213312</v>
       </c>
       <c r="D470" s="3">
-        <v>0</v>
+        <v>3102</v>
       </c>
     </row>
     <row r="471" spans="1:4">
@@ -8493,7 +8493,7 @@
         <v>26756253696</v>
       </c>
       <c r="D471" s="3">
-        <v>0</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="472" spans="1:4">
@@ -8507,7 +8507,7 @@
         <v>18415648768</v>
       </c>
       <c r="D472" s="3">
-        <v>0</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="473" spans="1:4">
@@ -8521,7 +8521,7 @@
         <v>41595117568</v>
       </c>
       <c r="D473" s="3">
-        <v>0</v>
+        <v>675</v>
       </c>
     </row>
     <row r="474" spans="1:4">
@@ -8535,7 +8535,7 @@
         <v>186823049216</v>
       </c>
       <c r="D474" s="3">
-        <v>0</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="475" spans="1:4">
@@ -8549,7 +8549,7 @@
         <v>120557051904</v>
       </c>
       <c r="D475" s="3">
-        <v>0</v>
+        <v>424</v>
       </c>
     </row>
     <row r="476" spans="1:4">
@@ -8563,7 +8563,7 @@
         <v>15779340288</v>
       </c>
       <c r="D476" s="3">
-        <v>1</v>
+        <v>15187</v>
       </c>
     </row>
     <row r="477" spans="1:4">
@@ -8577,7 +8577,7 @@
         <v>34376482816</v>
       </c>
       <c r="D477" s="3">
-        <v>0</v>
+        <v>6096</v>
       </c>
     </row>
     <row r="478" spans="1:4">
@@ -8591,7 +8591,7 @@
         <v>608999178240</v>
       </c>
       <c r="D478" s="3">
-        <v>0</v>
+        <v>630</v>
       </c>
     </row>
     <row r="479" spans="1:4">
@@ -8605,7 +8605,7 @@
         <v>54381719552</v>
       </c>
       <c r="D479" s="3">
-        <v>0</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="480" spans="1:4">
@@ -8619,7 +8619,7 @@
         <v>38050738176</v>
       </c>
       <c r="D480" s="3">
-        <v>0</v>
+        <v>689</v>
       </c>
     </row>
     <row r="481" spans="1:4">
@@ -8633,7 +8633,7 @@
         <v>24746600448</v>
       </c>
       <c r="D481" s="3">
-        <v>0</v>
+        <v>3079</v>
       </c>
     </row>
     <row r="482" spans="1:4">
@@ -8647,7 +8647,7 @@
         <v>58726092800</v>
       </c>
       <c r="D482" s="3">
-        <v>0</v>
+        <v>164</v>
       </c>
     </row>
     <row r="483" spans="1:4">
@@ -8661,7 +8661,7 @@
         <v>34484572160</v>
       </c>
       <c r="D483" s="3">
-        <v>0</v>
+        <v>990</v>
       </c>
     </row>
     <row r="484" spans="1:4">
@@ -8675,7 +8675,7 @@
         <v>7833428480</v>
       </c>
       <c r="D484" s="3">
-        <v>2</v>
+        <v>22040</v>
       </c>
     </row>
     <row r="485" spans="1:4">
@@ -8689,7 +8689,7 @@
         <v>743538098176</v>
       </c>
       <c r="D485" s="3">
-        <v>0</v>
+        <v>2149</v>
       </c>
     </row>
     <row r="486" spans="1:4">
@@ -8703,7 +8703,7 @@
         <v>212966064128</v>
       </c>
       <c r="D486" s="3">
-        <v>0</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="487" spans="1:4">
@@ -8717,7 +8717,7 @@
         <v>25709219840</v>
       </c>
       <c r="D487" s="3">
-        <v>1</v>
+        <v>18970</v>
       </c>
     </row>
     <row r="488" spans="1:4">
@@ -8731,7 +8731,7 @@
         <v>91696054272</v>
       </c>
       <c r="D488" s="3">
-        <v>0</v>
+        <v>871</v>
       </c>
     </row>
     <row r="489" spans="1:4">
@@ -8745,7 +8745,7 @@
         <v>22953050112</v>
       </c>
       <c r="D489" s="3">
-        <v>0</v>
+        <v>516</v>
       </c>
     </row>
     <row r="490" spans="1:4">
@@ -8759,7 +8759,7 @@
         <v>32211204096</v>
       </c>
       <c r="D490" s="3">
-        <v>0</v>
+        <v>1967</v>
       </c>
     </row>
     <row r="491" spans="1:4">
@@ -8773,7 +8773,7 @@
         <v>257069924352</v>
       </c>
       <c r="D491" s="3">
-        <v>0</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="492" spans="1:4">
@@ -8787,7 +8787,7 @@
         <v>86740697088</v>
       </c>
       <c r="D492" s="3">
-        <v>0</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="493" spans="1:4">
@@ -8801,7 +8801,7 @@
         <v>23586527232</v>
       </c>
       <c r="D493" s="3">
-        <v>0</v>
+        <v>610</v>
       </c>
     </row>
     <row r="494" spans="1:4">
@@ -8815,7 +8815,7 @@
         <v>25233225728</v>
       </c>
       <c r="D494" s="3">
-        <v>0</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="495" spans="1:4">
@@ -8829,7 +8829,7 @@
         <v>23504926720</v>
       </c>
       <c r="D495" s="3">
-        <v>0</v>
+        <v>6162</v>
       </c>
     </row>
     <row r="496" spans="1:4">
@@ -8843,7 +8843,7 @@
         <v>71336468480</v>
       </c>
       <c r="D496" s="3">
-        <v>0</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="497" spans="1:4">
@@ -8857,7 +8857,7 @@
         <v>32433451008</v>
       </c>
       <c r="D497" s="3">
-        <v>0</v>
+        <v>617</v>
       </c>
     </row>
     <row r="498" spans="1:4">
@@ -8871,7 +8871,7 @@
         <v>10364339200</v>
       </c>
       <c r="D498" s="3">
-        <v>0</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="499" spans="1:4">
@@ -8885,7 +8885,7 @@
         <v>41873723392</v>
       </c>
       <c r="D499" s="3">
-        <v>0</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="500" spans="1:4">
@@ -8899,7 +8899,7 @@
         <v>30793277440</v>
       </c>
       <c r="D500" s="3">
-        <v>0</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="501" spans="1:4">
@@ -8913,7 +8913,7 @@
         <v>38883053568</v>
       </c>
       <c r="D501" s="3">
-        <v>0</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="502" spans="1:4">
@@ -8927,7 +8927,7 @@
         <v>20993060864</v>
       </c>
       <c r="D502" s="3">
-        <v>0</v>
+        <v>488</v>
       </c>
     </row>
     <row r="503" spans="1:4">
@@ -8941,7 +8941,7 @@
         <v>22316195840</v>
       </c>
       <c r="D503" s="3">
-        <v>0</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="504" spans="1:4">
@@ -8955,7 +8955,7 @@
         <v>79738920960</v>
       </c>
       <c r="D504" s="3">
-        <v>0</v>
+        <v>1134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>